<commit_message>
Update set this->db to static::$db
</commit_message>
<xml_diff>
--- a/form/Stock 01-06-18/225.xlsx
+++ b/form/Stock 01-06-18/225.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppServ\www\erp_mvc\form\Stock 01-06-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70771ABC-E689-43C7-BC38-FEB316D9F2B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0F0246DB-608D-429E-9C0D-2213C1945202}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CFDA9B55-ED6C-4526-9668-9290C117FD33}"/>
   </bookViews>
@@ -471,15 +471,6 @@
     <t>ARNO-171202</t>
   </si>
   <si>
-    <t>ARNO-171203</t>
-  </si>
-  <si>
-    <t>ARNO-180119</t>
-  </si>
-  <si>
-    <t>ARNO-180151</t>
-  </si>
-  <si>
     <t>ARNO-180301</t>
   </si>
   <si>
@@ -499,6 +490,15 @@
   </si>
   <si>
     <t>price_total</t>
+  </si>
+  <si>
+    <t>ARNO-180151-</t>
+  </si>
+  <si>
+    <t>ARNO-180119-</t>
+  </si>
+  <si>
+    <t>ARNO-171203-</t>
   </si>
 </sst>
 </file>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19ED7249-B17A-48A2-941C-AA3E3E400A3C}">
   <dimension ref="A1:G492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="H157" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18" customHeight="1"/>
@@ -912,16 +912,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1">
@@ -2998,7 +2998,7 @@
     </row>
     <row r="150" spans="1:4" ht="18" customHeight="1">
       <c r="A150" s="4" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B150" s="1">
         <v>1</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="151" spans="1:4" ht="18" customHeight="1">
       <c r="A151" s="4" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B151" s="1">
         <v>3</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="152" spans="1:4" ht="18" customHeight="1">
       <c r="A152" s="4" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B152" s="1">
         <v>2</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="153" spans="1:4" ht="18" customHeight="1">
       <c r="A153" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B153" s="1">
         <v>2</v>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="154" spans="1:4" ht="18" customHeight="1">
       <c r="A154" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B154" s="1">
         <v>1</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="155" spans="1:4" ht="18" customHeight="1">
       <c r="A155" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B155" s="1">
         <v>1</v>

</xml_diff>